<commit_message>
Presentacion y memoria modificada
</commit_message>
<xml_diff>
--- a/Gestion/Diagramas/diagramaGant.xlsx
+++ b/Gestion/Diagramas/diagramaGant.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\ProyectoSoftware\PS01\Gestion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\PS01\Gestion\Diagramas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{596F926B-77C7-44B9-951D-3D0FEDD4E0E9}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C84F08E-F996-47D2-BAED-1113B929E871}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1368" windowWidth="23040" windowHeight="8316" xr2:uid="{67D9C62D-CC8C-4C23-AB6F-2AB5C16DFF27}"/>
+    <workbookView xWindow="0" yWindow="1824" windowWidth="23040" windowHeight="8316" xr2:uid="{67D9C62D-CC8C-4C23-AB6F-2AB5C16DFF27}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>1.-Analisis de requisitos</t>
   </si>
@@ -95,12 +95,18 @@
   <si>
     <t>3.4.- Despliegue, documentación</t>
   </si>
+  <si>
+    <t>Significado</t>
+  </si>
+  <si>
+    <t>Rombo</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -110,25 +116,15 @@
     </font>
     <font>
       <b/>
+      <u/>
       <sz val="11"/>
-      <color theme="5"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF92D050"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -154,7 +150,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
@@ -167,9 +163,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -197,10 +202,10 @@
       <xdr:rowOff>30480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>60960</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>167640</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>541020</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -215,8 +220,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3147060" y="1676400"/>
-          <a:ext cx="472440" cy="137160"/>
+          <a:off x="3390900" y="1676400"/>
+          <a:ext cx="388620" cy="152400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -252,13 +257,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>541020</xdr:colOff>
+      <xdr:colOff>548640</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>22860</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>213360</xdr:colOff>
+      <xdr:colOff>220980</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -275,7 +280,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3779520" y="1851660"/>
+          <a:off x="3787140" y="1851660"/>
           <a:ext cx="236220" cy="160020"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -318,9 +323,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>312420</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>144780</xdr:rowOff>
+      <xdr:rowOff>160020</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -336,7 +341,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4030980" y="2202180"/>
-          <a:ext cx="335280" cy="137160"/>
+          <a:ext cx="647700" cy="152400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -372,15 +377,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>15240</xdr:colOff>
+      <xdr:colOff>556260</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>563880</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>525780</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -395,8 +400,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4381500" y="2415540"/>
-          <a:ext cx="548640" cy="114300"/>
+          <a:off x="4922520" y="2385060"/>
+          <a:ext cx="1104900" cy="190500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -431,16 +436,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>586740</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>144780</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>15240</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>91440</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>175260</xdr:rowOff>
+      <xdr:rowOff>167640</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -455,8 +460,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4953000" y="2598420"/>
-          <a:ext cx="640080" cy="137160"/>
+          <a:off x="6187440" y="2552700"/>
+          <a:ext cx="403860" cy="175260"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -491,16 +496,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>320040</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>22860</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>30480</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>251460</xdr:colOff>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>167640</xdr:rowOff>
+      <xdr:rowOff>175260</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -515,8 +520,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5821680" y="2773680"/>
-          <a:ext cx="472440" cy="137160"/>
+          <a:off x="6598920" y="2758440"/>
+          <a:ext cx="1325880" cy="160020"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -552,15 +557,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>411480</xdr:colOff>
+      <xdr:colOff>281940</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>15240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>182880</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>175260</xdr:rowOff>
+      <xdr:colOff>175260</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -575,8 +580,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4213860" y="3147060"/>
-          <a:ext cx="335280" cy="137160"/>
+          <a:off x="4084320" y="3124200"/>
+          <a:ext cx="457200" cy="167640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -611,16 +616,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>213360</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>182880</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>510540</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>160020</xdr:rowOff>
+      <xdr:rowOff>175260</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -635,8 +640,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5181600" y="3299460"/>
-          <a:ext cx="434340" cy="152400"/>
+          <a:off x="4549140" y="3307080"/>
+          <a:ext cx="2004060" cy="160020"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -671,16 +676,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>281940</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>22860</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>236220</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -695,8 +700,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5783580" y="3680460"/>
-          <a:ext cx="1958340" cy="129540"/>
+          <a:off x="7658100" y="3672840"/>
+          <a:ext cx="1577340" cy="175260"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -731,16 +736,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>259080</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>251460</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>213360</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>175260</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -755,8 +760,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7764780" y="3840480"/>
-          <a:ext cx="929640" cy="175260"/>
+          <a:off x="4617720" y="3840480"/>
+          <a:ext cx="5387340" cy="198120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -791,16 +796,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>175260</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>15240</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>22860</xdr:rowOff>
+      <xdr:rowOff>7620</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>320040</xdr:colOff>
+      <xdr:colOff>495300</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>30480</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -815,8 +820,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8656320" y="5143500"/>
-          <a:ext cx="1668780" cy="190500"/>
+          <a:off x="10020300" y="5128260"/>
+          <a:ext cx="480060" cy="175260"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -854,11 +859,11 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>152400</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>99060</xdr:rowOff>
+      <xdr:rowOff>106680</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>541020</xdr:colOff>
+      <xdr:colOff>548640</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>102870</xdr:rowOff>
     </xdr:to>
@@ -878,8 +883,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3390900" y="1744980"/>
-          <a:ext cx="388620" cy="186690"/>
+          <a:off x="3390900" y="1752600"/>
+          <a:ext cx="396240" cy="179070"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -916,7 +921,7 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>228600</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:rowOff>83820</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -934,7 +939,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3810000" y="1996440"/>
-          <a:ext cx="220980" cy="274320"/>
+          <a:ext cx="220980" cy="281940"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -962,16 +967,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>175260</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>548640</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>129540</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>106680</xdr:rowOff>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>297180</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -986,7 +991,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4183380" y="2369820"/>
+          <a:off x="4495800" y="2392680"/>
           <a:ext cx="167640" cy="114300"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -1016,15 +1021,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
+      <xdr:colOff>320040</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>144780</xdr:rowOff>
+      <xdr:rowOff>121920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
+      <xdr:colOff>548640</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:rowOff>129540</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1039,7 +1044,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4709160" y="2522220"/>
+          <a:off x="4686300" y="2499360"/>
           <a:ext cx="228600" cy="190500"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -1122,15 +1127,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>15240</xdr:colOff>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>274320</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>53340</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1141,15 +1146,12 @@
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="3" idx="2"/>
-          <a:endCxn id="8" idx="0"/>
-        </xdr:cNvCxnSpPr>
+        <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3897630" y="2011680"/>
-          <a:ext cx="483870" cy="1135380"/>
+          <a:off x="3859530" y="1988820"/>
+          <a:ext cx="217170" cy="1173480"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1177,16 +1179,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>22860</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>106680</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>213360</xdr:colOff>
+      <xdr:colOff>289560</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>83820</xdr:rowOff>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1197,14 +1199,12 @@
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:endCxn id="9" idx="1"/>
-        </xdr:cNvCxnSpPr>
+        <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4389120" y="3215640"/>
-          <a:ext cx="792480" cy="160020"/>
+          <a:off x="4335780" y="3284220"/>
+          <a:ext cx="320040" cy="121920"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1232,16 +1232,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>548640</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>167640</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>213360</xdr:colOff>
+      <xdr:colOff>144780</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>91440</xdr:rowOff>
+      <xdr:rowOff>83820</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1256,8 +1256,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4533900" y="4320540"/>
-          <a:ext cx="647700" cy="160020"/>
+          <a:off x="4351020" y="4351020"/>
+          <a:ext cx="160020" cy="121920"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1340,16 +1340,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>243840</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>99060</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>45720</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>15240</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>388620</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1364,7 +1364,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8724900" y="3939540"/>
+          <a:off x="11414760" y="3825240"/>
           <a:ext cx="274320" cy="1196340"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -1393,16 +1393,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>525780</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>30480</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>205740</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>259080</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>521970</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1413,14 +1413,12 @@
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:endCxn id="41" idx="0"/>
-        </xdr:cNvCxnSpPr>
+        <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5494020" y="2773680"/>
-          <a:ext cx="213360" cy="739140"/>
+          <a:off x="3497580" y="3749040"/>
+          <a:ext cx="262890" cy="739140"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1448,16 +1446,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>396240</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>175260</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>144780</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>121920</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>160020</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>388620</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1472,7 +1470,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8397240" y="5113020"/>
+          <a:off x="10165080" y="4777740"/>
           <a:ext cx="228600" cy="129540"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -1561,16 +1559,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>213360</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>160020</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>518160</xdr:colOff>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>91440</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>160020</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1585,8 +1583,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5181600" y="4389120"/>
-          <a:ext cx="411480" cy="160020"/>
+          <a:off x="4526280" y="4381500"/>
+          <a:ext cx="2034540" cy="190500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1621,16 +1619,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>121920</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>525780</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:rowOff>160020</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1645,8 +1643,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5623560" y="4572000"/>
-          <a:ext cx="144780" cy="152400"/>
+          <a:off x="6568440" y="4594860"/>
+          <a:ext cx="1089660" cy="137160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1681,16 +1679,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>137160</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>15240</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>274320</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>160020</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>144780</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1704,9 +1702,9 @@
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5638800" y="3512820"/>
-          <a:ext cx="137160" cy="121920"/>
+        <a:xfrm flipV="1">
+          <a:off x="6591300" y="3474720"/>
+          <a:ext cx="1059180" cy="182880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1741,16 +1739,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>297180</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>175260</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>15240</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>129540</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>167640</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1765,8 +1763,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5798820" y="4770120"/>
-          <a:ext cx="1836420" cy="152400"/>
+          <a:off x="7680960" y="4747260"/>
+          <a:ext cx="1615440" cy="205740"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1801,16 +1799,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>137160</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>167640</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>160020</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>312420</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>502920</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>7620</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1825,8 +1823,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7642860" y="4922520"/>
-          <a:ext cx="998220" cy="198120"/>
+          <a:off x="4678680" y="4953000"/>
+          <a:ext cx="5318760" cy="175260"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1861,16 +1859,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>346710</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>175260</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>194310</xdr:colOff>
+      <xdr:rowOff>167640</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>22860</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1888,8 +1886,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5273040" y="2735580"/>
-          <a:ext cx="422910" cy="1836420"/>
+          <a:off x="6389370" y="2727960"/>
+          <a:ext cx="723900" cy="1866900"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1917,16 +1915,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>251460</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>365760</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>259080</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>87630</xdr:rowOff>
+      <xdr:rowOff>99060</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1942,9 +1940,9 @@
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7383780" y="3810000"/>
-          <a:ext cx="381000" cy="118110"/>
+        <a:xfrm flipH="1">
+          <a:off x="4617720" y="3810000"/>
+          <a:ext cx="2766060" cy="129540"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1972,16 +1970,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>312420</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>160020</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>167640</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>137160</xdr:colOff>
+      <xdr:colOff>167640</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>83820</xdr:rowOff>
+      <xdr:rowOff>102870</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1997,9 +1995,9 @@
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7178040" y="4922520"/>
-          <a:ext cx="464820" cy="99060"/>
+        <a:xfrm flipH="1">
+          <a:off x="4678680" y="4953000"/>
+          <a:ext cx="2506980" cy="87630"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -2027,16 +2025,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>53340</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>175260</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>297180</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>91440</xdr:rowOff>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2053,8 +2051,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5676900" y="4754880"/>
-          <a:ext cx="121920" cy="91440"/>
+          <a:off x="7559040" y="4732020"/>
+          <a:ext cx="121920" cy="118110"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -2082,332 +2080,766 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>294098</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>116035</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>551723</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>127805</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="55" name="Rombo 54" descr="l&#10;">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2A5EA89B-B48F-4CD7-B267-55AF301471AC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4660358" y="2310595"/>
+          <a:ext cx="257625" cy="194650"/>
+        </a:xfrm>
+        <a:prstGeom prst="diamond">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>reu</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>449580</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>144780</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="65" name="Rombo 64">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{23A1FE4B-5493-467C-ADD8-F4DD4524AC2C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6134100" y="2552700"/>
+          <a:ext cx="304800" cy="175260"/>
+        </a:xfrm>
+        <a:prstGeom prst="diamond">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-ES" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>449580</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>175260</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="66" name="Rombo 65">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D9002195-1854-408F-8B22-33CA3CD2CF18}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10546080" y="4084320"/>
+          <a:ext cx="236220" cy="175260"/>
+        </a:xfrm>
+        <a:prstGeom prst="diamond">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-ES" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>350520</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="68" name="Rombo 67">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{40028AE3-C454-41C3-BE38-EBEFCF604A89}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8221980" y="3505200"/>
+          <a:ext cx="236220" cy="175260"/>
+        </a:xfrm>
+        <a:prstGeom prst="diamond">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-ES" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>198120</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>434340</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="69" name="Rombo 68">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A37AEEA5-1DC9-4232-BF69-8070BDD6D494}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8305800" y="4594860"/>
+          <a:ext cx="236220" cy="175260"/>
+        </a:xfrm>
+        <a:prstGeom prst="diamond">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-ES" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>243840</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>480060</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="70" name="Rombo 69">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D89BB4A1-D9F2-4B70-98F3-3E18BABD3DCB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10340340" y="5196840"/>
+          <a:ext cx="236220" cy="175260"/>
+        </a:xfrm>
+        <a:prstGeom prst="diamond">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-ES" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>464820</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>15240</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>160020</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>15240</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>22860</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="67" name="Conector recto 66">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E150A1A8-3909-4150-9D0E-A8F54C940225}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6591300" y="1257300"/>
-          <a:ext cx="0" cy="4434840"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="19050">
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="72" name="Rombo 71">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EC0FFBB6-CAFD-402D-B263-46089B9D98B6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6758940" y="3459480"/>
+          <a:ext cx="236220" cy="175260"/>
+        </a:xfrm>
+        <a:prstGeom prst="diamond">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
           <a:solidFill>
             <a:schemeClr val="accent2"/>
           </a:solidFill>
         </a:ln>
       </xdr:spPr>
       <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>7620</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>15240</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>175260</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="71" name="Conector recto 70">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{389ED02C-2AE1-4D1A-9119-6DC47991B680}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="10515600" y="1287780"/>
-          <a:ext cx="7620" cy="4373880"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="19050">
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-ES" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>312420</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>548640</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="74" name="Rombo 73">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{14E9D190-6381-48D8-8194-31FF8E5217D1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6606540" y="4632960"/>
+          <a:ext cx="236220" cy="175260"/>
+        </a:xfrm>
+        <a:prstGeom prst="diamond">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
           <a:solidFill>
             <a:schemeClr val="accent2"/>
           </a:solidFill>
         </a:ln>
       </xdr:spPr>
       <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>175260</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>7620</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="73" name="Conector recto 72">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63C8B6E3-CFAA-40AD-AC2B-A3F23ADD1B5E}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="4968240" y="1272540"/>
-          <a:ext cx="7620" cy="4434840"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="28575">
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-ES" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>434340</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>670560</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="75" name="Rombo 74">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FDBA04A5-D8CB-45C4-AE9A-DF2EB93DA231}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6728460" y="2758440"/>
+          <a:ext cx="236220" cy="175260"/>
+        </a:xfrm>
+        <a:prstGeom prst="diamond">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
           <a:solidFill>
-            <a:srgbClr val="92D050"/>
+            <a:schemeClr val="accent2"/>
           </a:solidFill>
         </a:ln>
       </xdr:spPr>
       <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>160020</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>22860</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="77" name="Conector recto 76">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{02566C42-C3EE-4CFC-97AC-771AB5AE5B01}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="6035040" y="1257300"/>
-          <a:ext cx="30480" cy="4488180"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="28575">
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-ES" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="76" name="Rombo 75">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F92FD06B-8113-4B49-98D9-7DC08F15B001}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11102340" y="5257800"/>
+          <a:ext cx="236220" cy="175260"/>
+        </a:xfrm>
+        <a:prstGeom prst="diamond">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
           <a:solidFill>
-            <a:srgbClr val="92D050"/>
+            <a:schemeClr val="accent2"/>
           </a:solidFill>
         </a:ln>
       </xdr:spPr>
       <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>220980</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>175260</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>251460</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>175260</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="79" name="Conector recto 78">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{53E303DB-0D9F-43FC-BD95-086E070130E0}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="7726680" y="1455420"/>
-          <a:ext cx="30480" cy="4206240"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="28575">
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-ES" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>83820</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>320040</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="78" name="Rombo 77">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E4F530DA-23A8-4268-82C9-5CFE32EAEB2B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2849880" y="6408420"/>
+          <a:ext cx="236220" cy="175260"/>
+        </a:xfrm>
+        <a:prstGeom prst="diamond">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-ES" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>99060</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>335280</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="80" name="Rombo 79">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{30F09E2A-61B8-4316-89C2-E6C51E408EAA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2865120" y="6225540"/>
+          <a:ext cx="236220" cy="175260"/>
+        </a:xfrm>
+        <a:prstGeom prst="diamond">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
           <a:solidFill>
-            <a:srgbClr val="92D050"/>
+            <a:schemeClr val="accent2"/>
           </a:solidFill>
         </a:ln>
       </xdr:spPr>
       <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>502920</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>30480</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>7620</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>15240</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="86" name="Conector recto 85">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{21EAFC85-268D-47F8-91AF-4A75E2903626}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="9997440" y="1310640"/>
-          <a:ext cx="15240" cy="4373880"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="28575">
-          <a:solidFill>
-            <a:srgbClr val="92D050"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-ES" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -2710,22 +3142,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB4E67E8-B2E3-456D-A8C0-3FEB543E5283}">
-  <dimension ref="B8:Q35"/>
+  <dimension ref="B8:Q36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="U42" sqref="U42"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="31" customWidth="1"/>
-    <col min="3" max="3" width="4.6640625" customWidth="1"/>
+    <col min="2" max="2" width="28.77734375" customWidth="1"/>
+    <col min="3" max="3" width="6.5546875" customWidth="1"/>
     <col min="4" max="5" width="8.21875" customWidth="1"/>
-    <col min="6" max="6" width="8.77734375" customWidth="1"/>
-    <col min="7" max="7" width="7.77734375" customWidth="1"/>
-    <col min="8" max="8" width="7.88671875" customWidth="1"/>
-    <col min="9" max="9" width="7.77734375" customWidth="1"/>
-    <col min="10" max="10" width="6.44140625" customWidth="1"/>
+    <col min="6" max="6" width="9.88671875" customWidth="1"/>
+    <col min="7" max="7" width="9.33203125" customWidth="1"/>
+    <col min="8" max="8" width="8.88671875" customWidth="1"/>
+    <col min="9" max="9" width="10" customWidth="1"/>
+    <col min="10" max="10" width="9.33203125" customWidth="1"/>
     <col min="11" max="11" width="7.109375" customWidth="1"/>
     <col min="12" max="12" width="7.21875" customWidth="1"/>
     <col min="13" max="13" width="7" customWidth="1"/>
@@ -2924,22 +3356,36 @@
         <v>18</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B33" s="8" t="s">
         <v>19</v>
       </c>
+      <c r="C33" s="8"/>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B34" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B35" s="9" t="s">
         <v>20</v>
       </c>
+      <c r="C35" s="7"/>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B35" s="7" t="s">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B36" s="9" t="s">
         <v>21</v>
       </c>
+      <c r="C36" s="7"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B33:C33"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>